<commit_message>
Updates on RecruitOn: filters and maps
</commit_message>
<xml_diff>
--- a/files/template.xlsx
+++ b/files/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMS\Desktop\HACKING\WEB-DEVELOPMENT\TYPESCRIPT\PROJECTS\recruitment-manager-mvc\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A29AFE-C4F3-4D3E-8E07-A23125D35ED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762BCC9-8027-4320-8118-1F4CAF18B005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1170" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -52,9 +52,6 @@
     <t>ivanmist90@gmail.com</t>
   </si>
   <si>
-    <t>Málaga, Spain</t>
-  </si>
-  <si>
     <t>invented1@gmail.com</t>
   </si>
   <si>
@@ -92,6 +89,54 @@
   </si>
   <si>
     <t>Mkna2tremendo</t>
+  </si>
+  <si>
+    <t>Cádiz</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Málaga</t>
+  </si>
+  <si>
+    <t>Cinco</t>
+  </si>
+  <si>
+    <t>Cincel</t>
+  </si>
+  <si>
+    <t>Seis</t>
+  </si>
+  <si>
+    <t>Sesos</t>
+  </si>
+  <si>
+    <t>Siete</t>
+  </si>
+  <si>
+    <t>Mesino</t>
+  </si>
+  <si>
+    <t>Octavo</t>
+  </si>
+  <si>
+    <t>Del Ocho</t>
+  </si>
+  <si>
+    <t>cinco@cinco.com</t>
+  </si>
+  <si>
+    <t>seis@seis.com</t>
+  </si>
+  <si>
+    <t>siete@siete.com</t>
+  </si>
+  <si>
+    <t>oito@orto.com</t>
   </si>
 </sst>
 </file>
@@ -483,14 +528,14 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -517,12 +562,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -534,7 +579,7 @@
         <v>652710409</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2">
         <v>29</v>
@@ -546,111 +591,222 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2">
         <v>29</v>
       </c>
       <c r="H3" s="2">
-        <v>16800</v>
+        <v>16900</v>
       </c>
       <c r="I3" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2">
         <v>29</v>
       </c>
       <c r="H4" s="2">
-        <v>16800</v>
+        <v>16400</v>
       </c>
       <c r="I4" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="2">
         <v>600600644</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2">
         <v>29</v>
       </c>
       <c r="H5" s="2">
-        <v>16800</v>
+        <v>19000</v>
       </c>
       <c r="I5" s="2">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2">
+        <v>600600666</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2">
+        <v>12340</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2">
+        <v>600600665</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="2">
+        <v>29</v>
+      </c>
+      <c r="H7" s="2">
+        <v>15700</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2">
+        <v>600600610</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2">
+        <v>29</v>
+      </c>
+      <c r="H8" s="2">
+        <v>19230</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6.34</v>
+      </c>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2">
+        <v>600600669</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2">
+        <v>29</v>
+      </c>
+      <c r="H9" s="2">
+        <v>24800</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.8800000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{2CD021AB-CD78-45BD-A2F4-B5096D6CF841}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{91F4B145-3F2B-4B4E-9849-DF434907DD93}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{A2DA79D5-A48A-4C5F-84BE-EF811D8B7C06}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{1316D7CF-FEA2-4BC0-9D05-5570020E61CB}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{AC8E7ECC-A016-4F98-9677-8E57E5DEDB6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>